<commit_message>
Ignore DNB records without dates
</commit_message>
<xml_diff>
--- a/record/dnb/testdata/test.xlsx
+++ b/record/dnb/testdata/test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Dato</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Transaction 3</t>
+  </si>
+  <si>
+    <t>Transaction 4</t>
   </si>
 </sst>
 </file>
@@ -66,15 +69,21 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -84,16 +93,103 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -103,23 +199,50 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -139,6 +262,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -290,9 +414,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -372,7 +496,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -400,10 +524,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -659,9 +783,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -949,7 +1073,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -977,10 +1101,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1234,7 +1358,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1318,6 +1442,70 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" ht="15.35" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" ht="15.35" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" ht="15.35" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" ht="15.35" customHeight="1">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>